<commit_message>
Removed time slot validation when virtual days are 0
</commit_message>
<xml_diff>
--- a/spec/support/roInvalidNumberOfTimeSlots.xlsx
+++ b/spec/support/roInvalidNumberOfTimeSlots.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephenhalliburton/workspace/caseflow/spec/support/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D83F96ED-A023-8649-93B5-69FF3681F8C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20511B1E-D527-5F47-BA60-F6DDFDFD8FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13040" yWindow="460" windowWidth="25360" windowHeight="17440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="130">
   <si>
     <t>Example</t>
   </si>
@@ -6341,8 +6341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:IV98"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6557,17 +6557,11 @@
         <v>4</v>
       </c>
       <c r="E8" s="51">
-        <v>4</v>
-      </c>
-      <c r="F8" s="29">
-        <v>5</v>
-      </c>
-      <c r="G8" s="29">
-        <v>30</v>
-      </c>
-      <c r="H8" s="76" t="s">
-        <v>128</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="76"/>
       <c r="I8" s="29"/>
       <c r="J8" s="29"/>
       <c r="K8" s="29"/>

</xml_diff>